<commit_message>
Adding the consideration of the decay chain
</commit_message>
<xml_diff>
--- a/Yield_Comparison_v2_add_FRMII.xlsx
+++ b/Yield_Comparison_v2_add_FRMII.xlsx
@@ -8,21 +8,22 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\myDataBase\cyanus\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D9502592-2CBD-470E-AD60-A1977C9FA92A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9D733021-D65E-4F18-B358-656F0732936A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="element" sheetId="1" r:id="rId1"/>
     <sheet name="简明" sheetId="3" r:id="rId2"/>
     <sheet name="简明-论文用" sheetId="5" r:id="rId3"/>
+    <sheet name="简明-论文用 (2)" sheetId="6" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1596" uniqueCount="756">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2035" uniqueCount="761">
   <si>
     <t>element</t>
   </si>
@@ -2523,6 +2524,26 @@
   </si>
   <si>
     <t>Ir192m</t>
+  </si>
+  <si>
+    <t>Sm155</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Sm155</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tm170</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Tm170</t>
+    <phoneticPr fontId="18" type="noConversion"/>
+  </si>
+  <si>
+    <t>Ir192m</t>
+    <phoneticPr fontId="18" type="noConversion"/>
   </si>
 </sst>
 </file>
@@ -2981,7 +3002,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="13">
     <border>
       <left/>
       <right/>
@@ -3112,6 +3133,15 @@
         <color indexed="64"/>
       </top>
       <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
       <diagonal/>
     </border>
   </borders>
@@ -3246,7 +3276,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="64">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -3425,6 +3455,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="19" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="12" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="21" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="19" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="25" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -3786,10 +3828,10 @@
   <dimension ref="A1:AF85"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="4" ySplit="9" topLeftCell="E69" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="4" ySplit="9" topLeftCell="J10" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="A76" sqref="A76:XFD76"/>
+      <selection pane="bottomRight" activeCell="V73" sqref="V73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -4123,6 +4165,10 @@
         <f>S10*T10</f>
         <v>45264.799999999996</v>
       </c>
+      <c r="V10" s="1">
+        <f>ABS(I10-U10)/U10</f>
+        <v>1.3771186440650449E-4</v>
+      </c>
       <c r="W10" t="s">
         <v>328</v>
       </c>
@@ -4195,6 +4241,10 @@
         <f t="shared" ref="U11:U74" si="1">S11*T11</f>
         <v>1309886030</v>
       </c>
+      <c r="V11" s="1">
+        <f t="shared" ref="V11:V74" si="2">ABS(I11-U11)/U11</f>
+        <v>1.0260663670105712E-3</v>
+      </c>
       <c r="W11" t="s">
         <v>329</v>
       </c>
@@ -4266,6 +4316,10 @@
         <f t="shared" si="1"/>
         <v>162855000</v>
       </c>
+      <c r="V12" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8115501519756839E-3</v>
+      </c>
       <c r="W12" t="s">
         <v>330</v>
       </c>
@@ -4340,6 +4394,10 @@
         <f t="shared" si="1"/>
         <v>2690000000</v>
       </c>
+      <c r="V13" s="1">
+        <f t="shared" si="2"/>
+        <v>9.2193308550185879E-5</v>
+      </c>
       <c r="W13" t="s">
         <v>331</v>
       </c>
@@ -4411,6 +4469,10 @@
         <f t="shared" si="1"/>
         <v>272122000</v>
       </c>
+      <c r="V14" s="1">
+        <f t="shared" si="2"/>
+        <v>2.6912928759894461E-4</v>
+      </c>
       <c r="W14" t="s">
         <v>332</v>
       </c>
@@ -4497,6 +4559,10 @@
         <f t="shared" si="1"/>
         <v>22300000000</v>
       </c>
+      <c r="V15" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0950672645739911E-3</v>
+      </c>
       <c r="W15" t="s">
         <v>333</v>
       </c>
@@ -4583,6 +4649,10 @@
         <f t="shared" si="1"/>
         <v>36730.200000000004</v>
       </c>
+      <c r="V16" s="1">
+        <f t="shared" si="2"/>
+        <v>0.26855013041039777</v>
+      </c>
       <c r="W16" t="s">
         <v>334</v>
       </c>
@@ -4660,6 +4730,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V17" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
     </row>
     <row r="18" spans="1:32" x14ac:dyDescent="0.25">
       <c r="A18" t="s">
@@ -4684,7 +4758,7 @@
         <v>0.94</v>
       </c>
       <c r="I18" s="1">
-        <f t="shared" ref="I18:I59" si="2">G18/1000000*37000000000*H18</f>
+        <f t="shared" ref="I18:I59" si="3">G18/1000000*37000000000*H18</f>
         <v>1521103.2999999998</v>
       </c>
       <c r="K18" s="4" t="s">
@@ -4716,6 +4790,10 @@
         <f t="shared" si="1"/>
         <v>0</v>
       </c>
+      <c r="V18" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#DIV/0!</v>
+      </c>
       <c r="W18" t="s">
         <v>335</v>
       </c>
@@ -4767,7 +4845,7 @@
         <v>0.42399999999999999</v>
       </c>
       <c r="I19" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2047911520</v>
       </c>
       <c r="K19" t="s">
@@ -4802,6 +4880,10 @@
         <f t="shared" si="1"/>
         <v>2125200000</v>
       </c>
+      <c r="V19" s="1">
+        <f t="shared" si="2"/>
+        <v>3.6367626576322226E-2</v>
+      </c>
       <c r="W19" t="s">
         <v>336</v>
       </c>
@@ -4853,7 +4935,7 @@
         <v>0.99099999999999999</v>
       </c>
       <c r="I20" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>13297287549.999998</v>
       </c>
       <c r="K20" t="s">
@@ -4888,6 +4970,10 @@
         <f t="shared" si="1"/>
         <v>13287440000</v>
       </c>
+      <c r="V20" s="1">
+        <f t="shared" si="2"/>
+        <v>7.411171753172991E-4</v>
+      </c>
       <c r="W20" t="s">
         <v>337</v>
       </c>
@@ -4939,7 +5025,7 @@
         <v>0.18</v>
       </c>
       <c r="I21" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>60655950</v>
       </c>
       <c r="K21" t="s">
@@ -4974,6 +5060,10 @@
         <f t="shared" si="1"/>
         <v>61110399.999999993</v>
       </c>
+      <c r="V21" s="1">
+        <f t="shared" si="2"/>
+        <v>7.436541079750625E-3</v>
+      </c>
       <c r="W21" t="s">
         <v>338</v>
       </c>
@@ -5025,7 +5115,7 @@
         <v>0.92</v>
       </c>
       <c r="I22" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>101929376</v>
       </c>
       <c r="K22" t="s">
@@ -5060,6 +5150,10 @@
         <f t="shared" si="1"/>
         <v>98884800</v>
       </c>
+      <c r="V22" s="1">
+        <f t="shared" si="2"/>
+        <v>3.0789120269242593E-2</v>
+      </c>
       <c r="W22" t="s">
         <v>339</v>
       </c>
@@ -5111,7 +5205,7 @@
         <v>0.62</v>
       </c>
       <c r="I23" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>349674420000</v>
       </c>
       <c r="K23" s="4" t="s">
@@ -5149,6 +5243,10 @@
         <f t="shared" si="1"/>
         <v>349680000000</v>
       </c>
+      <c r="V23" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5957446808510637E-5</v>
+      </c>
       <c r="W23" t="s">
         <v>340</v>
       </c>
@@ -5200,7 +5298,7 @@
         <v>0.93</v>
       </c>
       <c r="I24" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>456655110</v>
       </c>
       <c r="K24" s="2" t="s">
@@ -5223,6 +5321,10 @@
         <f t="shared" si="1"/>
         <v>446880000</v>
       </c>
+      <c r="V24" s="1">
+        <f t="shared" si="2"/>
+        <v>2.1874127282491943E-2</v>
+      </c>
       <c r="W24" t="s">
         <v>341</v>
       </c>
@@ -5274,7 +5376,7 @@
         <v>1</v>
       </c>
       <c r="I25" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>249720400000</v>
       </c>
       <c r="K25" s="2" t="s">
@@ -5298,6 +5400,10 @@
         <f t="shared" si="1"/>
         <v>250000000000</v>
       </c>
+      <c r="V25" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1184000000000001E-3</v>
+      </c>
       <c r="W25" t="s">
         <v>342</v>
       </c>
@@ -5349,7 +5455,7 @@
         <v>3.6999999999999999E-4</v>
       </c>
       <c r="I26" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>150767.97</v>
       </c>
       <c r="K26" t="s">
@@ -5365,7 +5471,7 @@
         <v>0.1</v>
       </c>
       <c r="O26" s="1">
-        <f t="shared" ref="O26:O45" si="3">M26*N26</f>
+        <f t="shared" ref="O26:O45" si="4">M26*N26</f>
         <v>3586000</v>
       </c>
       <c r="Q26" t="s">
@@ -5384,6 +5490,10 @@
         <f t="shared" si="1"/>
         <v>150960</v>
       </c>
+      <c r="V26" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2720588235294041E-3</v>
+      </c>
       <c r="W26" t="s">
         <v>343</v>
       </c>
@@ -5435,7 +5545,7 @@
         <v>0.98899999999999999</v>
       </c>
       <c r="I27" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>145925565400</v>
       </c>
       <c r="K27" t="s">
@@ -5451,7 +5561,7 @@
         <v>0.98899999999999999</v>
       </c>
       <c r="O27" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>146668700000</v>
       </c>
       <c r="Q27" t="s">
@@ -5470,6 +5580,10 @@
         <f t="shared" si="1"/>
         <v>146298000000</v>
       </c>
+      <c r="V27" s="1">
+        <f t="shared" si="2"/>
+        <v>2.5457258472432981E-3</v>
+      </c>
       <c r="W27" t="s">
         <v>344</v>
       </c>
@@ -5521,7 +5635,7 @@
         <v>1.2799999999999999E-9</v>
       </c>
       <c r="I28" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2.3477299200000003E-4</v>
       </c>
       <c r="K28" t="s">
@@ -5537,7 +5651,7 @@
         <v>1.2799999999999999E-9</v>
       </c>
       <c r="O28" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2.2656E-4</v>
       </c>
       <c r="Q28" t="s">
@@ -5556,6 +5670,10 @@
         <f t="shared" si="1"/>
         <v>2.3679999999999998E-4</v>
       </c>
+      <c r="V28" s="1">
+        <f t="shared" si="2"/>
+        <v>8.5599999999998056E-3</v>
+      </c>
       <c r="W28" s="4" t="s">
         <v>345</v>
       </c>
@@ -5607,7 +5725,7 @@
         <v>0.02</v>
       </c>
       <c r="I29" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>16190460000</v>
       </c>
       <c r="K29" s="4" t="s">
@@ -5623,7 +5741,7 @@
         <v>0.99982599999999999</v>
       </c>
       <c r="O29" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>24485738.739999998</v>
       </c>
       <c r="P29" t="s">
@@ -5645,6 +5763,10 @@
         <f t="shared" si="1"/>
         <v>16686000000</v>
       </c>
+      <c r="V29" s="1">
+        <f t="shared" si="2"/>
+        <v>2.9697950377562028E-2</v>
+      </c>
       <c r="W29" t="s">
         <v>346</v>
       </c>
@@ -5696,7 +5818,7 @@
         <v>0.24</v>
       </c>
       <c r="I30" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35054688</v>
       </c>
       <c r="K30" t="s">
@@ -5712,7 +5834,7 @@
         <v>0.24</v>
       </c>
       <c r="O30" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>37728000</v>
       </c>
       <c r="Q30" t="s">
@@ -5731,6 +5853,10 @@
         <f t="shared" si="1"/>
         <v>33497800</v>
       </c>
+      <c r="V30" s="1">
+        <f t="shared" si="2"/>
+        <v>4.6477320898685885E-2</v>
+      </c>
       <c r="W30" t="s">
         <v>347</v>
       </c>
@@ -5782,7 +5908,7 @@
         <v>0.09</v>
       </c>
       <c r="I31" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2403760500</v>
       </c>
       <c r="K31" t="s">
@@ -5798,7 +5924,7 @@
         <v>0.09</v>
       </c>
       <c r="O31" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>2450700000</v>
       </c>
       <c r="Q31" t="s">
@@ -5817,6 +5943,10 @@
         <f t="shared" si="1"/>
         <v>2455180000</v>
       </c>
+      <c r="V31" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0943270961803206E-2</v>
+      </c>
       <c r="W31" t="s">
         <v>348</v>
       </c>
@@ -5868,7 +5998,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="I32" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44555.4</v>
       </c>
       <c r="K32" t="s">
@@ -5884,7 +6014,7 @@
         <v>1.2E-5</v>
       </c>
       <c r="O32" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>3328.8</v>
       </c>
       <c r="Q32" t="s">
@@ -5903,6 +6033,10 @@
         <f t="shared" si="1"/>
         <v>44880</v>
       </c>
+      <c r="V32" s="1">
+        <f t="shared" si="2"/>
+        <v>7.2326203208555829E-3</v>
+      </c>
       <c r="W32" s="4" t="s">
         <v>349</v>
       </c>
@@ -5954,7 +6088,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
       <c r="I33" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>211661645</v>
       </c>
       <c r="K33" t="s">
@@ -5970,7 +6104,7 @@
         <v>6.4999999999999997E-3</v>
       </c>
       <c r="O33" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>209495000</v>
       </c>
       <c r="Q33" t="s">
@@ -5989,6 +6123,10 @@
         <f t="shared" si="1"/>
         <v>211900000</v>
       </c>
+      <c r="V33" s="1">
+        <f t="shared" si="2"/>
+        <v>1.1248466257668711E-3</v>
+      </c>
       <c r="W33" s="4" t="s">
         <v>350</v>
       </c>
@@ -6040,7 +6178,7 @@
         <v>0.114</v>
       </c>
       <c r="I34" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>291906690</v>
       </c>
       <c r="K34" s="4" t="s">
@@ -6056,7 +6194,7 @@
         <v>0.114</v>
       </c>
       <c r="O34" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>310308000</v>
       </c>
       <c r="Q34" s="47" t="s">
@@ -6075,6 +6213,10 @@
         <f t="shared" si="1"/>
         <v>290700000</v>
       </c>
+      <c r="V34" s="1">
+        <f t="shared" si="2"/>
+        <v>4.1509803921568628E-3</v>
+      </c>
       <c r="W34" s="4" t="s">
         <v>351</v>
       </c>
@@ -6126,7 +6268,7 @@
         <v>0.45</v>
       </c>
       <c r="I35" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1804027500</v>
       </c>
       <c r="K35" t="s">
@@ -6142,7 +6284,7 @@
         <v>0.45</v>
       </c>
       <c r="O35" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1708650000</v>
       </c>
       <c r="Q35" t="s">
@@ -6161,6 +6303,10 @@
         <f t="shared" si="1"/>
         <v>1804500000</v>
       </c>
+      <c r="V35" s="1">
+        <f t="shared" si="2"/>
+        <v>2.6184538653366583E-4</v>
+      </c>
       <c r="W35" t="s">
         <v>352</v>
       </c>
@@ -6212,7 +6358,7 @@
         <v>0.53</v>
       </c>
       <c r="I36" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>35760796000.000008</v>
       </c>
       <c r="K36" s="4" t="s">
@@ -6228,7 +6374,7 @@
         <v>6.7999999999999996E-3</v>
       </c>
       <c r="O36" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>60533600</v>
       </c>
       <c r="Q36" t="s">
@@ -6247,6 +6393,10 @@
         <f t="shared" si="1"/>
         <v>37346400000</v>
       </c>
+      <c r="V36" s="1">
+        <f t="shared" si="2"/>
+        <v>4.2456675877728306E-2</v>
+      </c>
       <c r="W36" t="s">
         <v>353</v>
       </c>
@@ -6298,7 +6448,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="I37" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>9011128000</v>
       </c>
       <c r="K37" t="s">
@@ -6314,7 +6464,7 @@
         <v>7.0000000000000007E-2</v>
       </c>
       <c r="O37" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>10773000000.000002</v>
       </c>
       <c r="Q37" t="s">
@@ -6333,6 +6483,10 @@
         <f t="shared" si="1"/>
         <v>8643000000</v>
       </c>
+      <c r="V37" s="1">
+        <f t="shared" si="2"/>
+        <v>4.2592618303829689E-2</v>
+      </c>
       <c r="W37" t="s">
         <v>354</v>
       </c>
@@ -6384,7 +6538,7 @@
         <v>5.5E-2</v>
       </c>
       <c r="I38" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>889457800</v>
       </c>
       <c r="K38" s="4" t="s">
@@ -6400,7 +6554,7 @@
         <v>0.127</v>
       </c>
       <c r="O38" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>1271270</v>
       </c>
       <c r="Q38" t="s">
@@ -6419,6 +6573,10 @@
         <f t="shared" si="1"/>
         <v>885500000</v>
       </c>
+      <c r="V38" s="1">
+        <f t="shared" si="2"/>
+        <v>4.4695652173913046E-3</v>
+      </c>
       <c r="W38" s="4" t="s">
         <v>355</v>
       </c>
@@ -6458,7 +6616,7 @@
         <v>0.98</v>
       </c>
       <c r="I39" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1142117480</v>
       </c>
       <c r="K39" s="4" t="s">
@@ -6474,7 +6632,7 @@
         <v>0.98</v>
       </c>
       <c r="O39" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>895230000</v>
       </c>
       <c r="Q39" t="s">
@@ -6493,6 +6651,10 @@
         <f t="shared" si="1"/>
         <v>1149057000</v>
       </c>
+      <c r="V39" s="1">
+        <f t="shared" si="2"/>
+        <v>6.0393174577066241E-3</v>
+      </c>
       <c r="W39" t="s">
         <v>356</v>
       </c>
@@ -6544,7 +6706,7 @@
         <v>0.81899999999999995</v>
       </c>
       <c r="I40" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>448363188</v>
       </c>
       <c r="K40" s="4" t="s">
@@ -6560,7 +6722,7 @@
         <v>9.5600000000000006E-5</v>
       </c>
       <c r="O40" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>7.7321280000000003</v>
       </c>
       <c r="Q40" t="s">
@@ -6579,6 +6741,10 @@
         <f t="shared" si="1"/>
         <v>447935500</v>
       </c>
+      <c r="V40" s="1">
+        <f t="shared" si="2"/>
+        <v>9.5479817964863243E-4</v>
+      </c>
       <c r="W40" t="s">
         <v>357</v>
       </c>
@@ -6630,7 +6796,7 @@
         <v>1.4E-8</v>
       </c>
       <c r="I41" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>5.6083859999999994</v>
       </c>
       <c r="K41" t="s">
@@ -6646,7 +6812,7 @@
         <v>1.4E-8</v>
       </c>
       <c r="O41" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>5.6181999999999999</v>
       </c>
       <c r="Q41" t="s">
@@ -6665,6 +6831,10 @@
         <f t="shared" si="1"/>
         <v>5.6139999999999999</v>
       </c>
+      <c r="V41" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0000000000000805E-3</v>
+      </c>
       <c r="W41" s="4" t="s">
         <v>358</v>
       </c>
@@ -6716,7 +6886,7 @@
         <v>0.93</v>
       </c>
       <c r="I42" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>653067.39</v>
       </c>
       <c r="K42" t="s">
@@ -6732,7 +6902,7 @@
         <v>0.93</v>
       </c>
       <c r="O42" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>585249</v>
       </c>
       <c r="Q42" t="s">
@@ -6751,6 +6921,10 @@
         <f t="shared" si="1"/>
         <v>653491.79999999993</v>
       </c>
+      <c r="V42" s="1">
+        <f t="shared" si="2"/>
+        <v>6.4944961818941911E-4</v>
+      </c>
       <c r="W42" t="s">
         <v>359</v>
       </c>
@@ -6802,7 +6976,7 @@
         <v>5.0000000000000001E-3</v>
       </c>
       <c r="I43" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>159928800</v>
       </c>
       <c r="K43" s="4" t="s">
@@ -6818,7 +6992,7 @@
         <v>0.99890000000000001</v>
       </c>
       <c r="O43" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>124.56283000000001</v>
       </c>
       <c r="Q43" t="s">
@@ -6837,6 +7011,10 @@
         <f t="shared" si="1"/>
         <v>160000000</v>
       </c>
+      <c r="V43" s="1">
+        <f t="shared" si="2"/>
+        <v>4.4499999999999997E-4</v>
+      </c>
       <c r="W43" t="s">
         <v>360</v>
       </c>
@@ -6888,7 +7066,7 @@
         <v>0.192</v>
       </c>
       <c r="I44" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>89489088</v>
       </c>
       <c r="K44" t="s">
@@ -6904,7 +7082,7 @@
         <v>0.192</v>
       </c>
       <c r="O44" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>93484800</v>
       </c>
       <c r="Q44" t="s">
@@ -6923,6 +7101,10 @@
         <f t="shared" si="1"/>
         <v>89856000</v>
       </c>
+      <c r="V44" s="1">
+        <f t="shared" si="2"/>
+        <v>4.0833333333333329E-3</v>
+      </c>
       <c r="W44" t="s">
         <v>361</v>
       </c>
@@ -6974,7 +7156,7 @@
         <v>0.47</v>
       </c>
       <c r="I45" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100689839</v>
       </c>
       <c r="K45" t="s">
@@ -6990,7 +7172,7 @@
         <v>0.47</v>
       </c>
       <c r="O45" s="1">
-        <f t="shared" si="3"/>
+        <f t="shared" si="4"/>
         <v>152891000</v>
       </c>
       <c r="Q45" t="s">
@@ -7009,6 +7191,10 @@
         <f t="shared" si="1"/>
         <v>102292000</v>
       </c>
+      <c r="V45" s="1">
+        <f t="shared" si="2"/>
+        <v>1.5662622687991241E-2</v>
+      </c>
       <c r="W45" t="s">
         <v>362</v>
       </c>
@@ -7060,7 +7246,7 @@
         <v>0.02</v>
       </c>
       <c r="I46" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>67888340000</v>
       </c>
       <c r="K46" s="2" t="s">
@@ -7084,6 +7270,10 @@
         <f t="shared" si="1"/>
         <v>67800000000</v>
       </c>
+      <c r="V46" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3029498525073747E-3</v>
+      </c>
       <c r="W46" t="s">
         <v>363</v>
       </c>
@@ -7135,7 +7325,7 @@
         <v>3.6700000000000003E-2</v>
       </c>
       <c r="I47" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>100050072.00000001</v>
       </c>
       <c r="K47" t="s">
@@ -7151,7 +7341,7 @@
         <v>3.6700000000000003E-2</v>
       </c>
       <c r="O47" s="1">
-        <f t="shared" ref="O47:O81" si="4">M47*N47</f>
+        <f t="shared" ref="O47:O81" si="5">M47*N47</f>
         <v>90318700.000000015</v>
       </c>
       <c r="Q47" t="s">
@@ -7170,6 +7360,10 @@
         <f t="shared" si="1"/>
         <v>99090000.000000015</v>
       </c>
+      <c r="V47" s="1">
+        <f t="shared" si="2"/>
+        <v>9.6888888888888875E-3</v>
+      </c>
       <c r="W47" s="4" t="s">
         <v>364</v>
       </c>
@@ -7221,7 +7415,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="I48" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>44447175000</v>
       </c>
       <c r="K48" t="s">
@@ -7237,7 +7431,7 @@
         <v>4.4999999999999998E-2</v>
       </c>
       <c r="O48" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>47295000000</v>
       </c>
       <c r="Q48" t="s">
@@ -7256,6 +7450,10 @@
         <f t="shared" si="1"/>
         <v>44460000000</v>
       </c>
+      <c r="V48" s="1">
+        <f t="shared" si="2"/>
+        <v>2.8846153846153849E-4</v>
+      </c>
       <c r="W48" t="s">
         <v>365</v>
       </c>
@@ -7307,7 +7505,7 @@
         <v>0.94</v>
       </c>
       <c r="I49" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>219781776</v>
       </c>
       <c r="K49" s="4" t="s">
@@ -7323,7 +7521,7 @@
         <v>0.32</v>
       </c>
       <c r="O49" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>10028800</v>
       </c>
       <c r="Q49" t="s">
@@ -7342,6 +7540,10 @@
         <f t="shared" si="1"/>
         <v>221840000</v>
       </c>
+      <c r="V49" s="1">
+        <f t="shared" si="2"/>
+        <v>9.277966101694915E-3</v>
+      </c>
       <c r="W49" t="s">
         <v>366</v>
       </c>
@@ -7393,7 +7595,7 @@
         <v>0.84399999999999997</v>
       </c>
       <c r="I50" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1585508016000</v>
       </c>
       <c r="K50" s="4" t="s">
@@ -7409,7 +7611,7 @@
         <v>1.4E-3</v>
       </c>
       <c r="O50" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16282000</v>
       </c>
       <c r="Q50" t="s">
@@ -7428,6 +7630,10 @@
         <f t="shared" si="1"/>
         <v>1594240000000</v>
       </c>
+      <c r="V50" s="1">
+        <f t="shared" si="2"/>
+        <v>5.4772079486150142E-3</v>
+      </c>
       <c r="W50" t="s">
         <v>367</v>
       </c>
@@ -7479,7 +7685,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="I51" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>151145902.79999998</v>
       </c>
       <c r="K51" s="4" t="s">
@@ -7495,7 +7701,7 @@
         <v>0.97199999999999998</v>
       </c>
       <c r="O51" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>24319440</v>
       </c>
       <c r="Q51" t="s">
@@ -7514,6 +7720,10 @@
         <f t="shared" si="1"/>
         <v>295089</v>
       </c>
+      <c r="V51" s="1">
+        <f t="shared" si="2"/>
+        <v>511.20446306029703</v>
+      </c>
       <c r="W51" t="s">
         <v>368</v>
       </c>
@@ -7565,7 +7775,7 @@
         <v>0.70679999999999998</v>
       </c>
       <c r="I52" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>544162492.79999995</v>
       </c>
       <c r="K52" t="s">
@@ -7581,7 +7791,7 @@
         <v>0.70679999999999998</v>
       </c>
       <c r="O52" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>540489960</v>
       </c>
       <c r="Q52" t="s">
@@ -7600,6 +7810,10 @@
         <f t="shared" si="1"/>
         <v>543452300</v>
       </c>
+      <c r="V52" s="1">
+        <f t="shared" si="2"/>
+        <v>1.3068171760427774E-3</v>
+      </c>
       <c r="W52" s="4" t="s">
         <v>369</v>
       </c>
@@ -7651,7 +7865,7 @@
         <v>0.69</v>
       </c>
       <c r="I53" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1037845559.9999999</v>
       </c>
       <c r="K53" t="s">
@@ -7667,7 +7881,7 @@
         <v>0.69</v>
       </c>
       <c r="O53" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1135050000</v>
       </c>
       <c r="Q53" t="s">
@@ -7686,6 +7900,10 @@
         <f t="shared" si="1"/>
         <v>1025119999.9999999</v>
       </c>
+      <c r="V53" s="1">
+        <f t="shared" si="2"/>
+        <v>1.2413727173404091E-2</v>
+      </c>
       <c r="W53" t="s">
         <v>370</v>
       </c>
@@ -7737,7 +7955,7 @@
         <v>0.17</v>
       </c>
       <c r="I54" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17423929000</v>
       </c>
       <c r="K54" t="s">
@@ -7753,7 +7971,7 @@
         <v>0.17</v>
       </c>
       <c r="O54" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17425000000</v>
       </c>
       <c r="Q54" t="s">
@@ -7772,6 +7990,10 @@
         <f t="shared" si="1"/>
         <v>117300000</v>
       </c>
+      <c r="V54" s="1">
+        <f t="shared" si="2"/>
+        <v>147.54159420289855</v>
+      </c>
       <c r="W54" t="s">
         <v>371</v>
       </c>
@@ -7823,7 +8045,7 @@
         <v>0.60199999999999998</v>
       </c>
       <c r="I55" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>337963402</v>
       </c>
       <c r="K55" s="4" t="s">
@@ -7839,7 +8061,7 @@
         <v>0.53800000000000003</v>
       </c>
       <c r="O55" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>69886200</v>
       </c>
       <c r="Q55" t="s">
@@ -7858,6 +8080,10 @@
         <f t="shared" si="1"/>
         <v>88894000</v>
       </c>
+      <c r="V55" s="1">
+        <f t="shared" si="2"/>
+        <v>2.8018696649942627</v>
+      </c>
       <c r="W55" s="4" t="s">
         <v>372</v>
       </c>
@@ -7897,7 +8123,7 @@
         <v>0.13</v>
       </c>
       <c r="I56" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>1349541700</v>
       </c>
       <c r="K56" s="4" t="s">
@@ -7913,7 +8139,7 @@
         <v>0.97619999999999996</v>
       </c>
       <c r="O56" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>22091406</v>
       </c>
       <c r="Q56" t="s">
@@ -7932,6 +8158,10 @@
         <f t="shared" si="1"/>
         <v>1310400000</v>
       </c>
+      <c r="V56" s="1">
+        <f t="shared" si="2"/>
+        <v>2.9870039682539682E-2</v>
+      </c>
       <c r="W56" t="s">
         <v>373</v>
       </c>
@@ -7983,7 +8213,7 @@
         <v>0.23699999999999999</v>
       </c>
       <c r="I57" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>450963363</v>
       </c>
       <c r="K57" t="s">
@@ -7999,7 +8229,7 @@
         <v>0.23699999999999999</v>
       </c>
       <c r="O57" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>511446000</v>
       </c>
       <c r="Q57" t="s">
@@ -8018,6 +8248,10 @@
         <f t="shared" si="1"/>
         <v>450300000</v>
       </c>
+      <c r="V57" s="1">
+        <f t="shared" si="2"/>
+        <v>1.473157894736842E-3</v>
+      </c>
       <c r="W57" t="s">
         <v>374</v>
       </c>
@@ -8069,7 +8303,7 @@
         <v>0.95399999999999996</v>
       </c>
       <c r="I58" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>2709650970</v>
       </c>
       <c r="K58" t="s">
@@ -8085,7 +8319,7 @@
         <v>0.95399999999999996</v>
       </c>
       <c r="O58" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>2739888000</v>
       </c>
       <c r="Q58" t="s">
@@ -8104,6 +8338,10 @@
         <f t="shared" si="1"/>
         <v>2709360000</v>
       </c>
+      <c r="V58" s="1">
+        <f t="shared" si="2"/>
+        <v>1.073943661971831E-4</v>
+      </c>
       <c r="W58" t="s">
         <v>375</v>
       </c>
@@ -8155,7 +8393,7 @@
         <v>0.42799999999999999</v>
       </c>
       <c r="I59" s="1">
-        <f t="shared" si="2"/>
+        <f t="shared" si="3"/>
         <v>17063289.999999996</v>
       </c>
       <c r="K59" t="s">
@@ -8171,7 +8409,7 @@
         <v>0.42799999999999999</v>
       </c>
       <c r="O59" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>17663560</v>
       </c>
       <c r="Q59" t="s">
@@ -8190,6 +8428,10 @@
         <f t="shared" si="1"/>
         <v>17120000</v>
       </c>
+      <c r="V59" s="1">
+        <f t="shared" si="2"/>
+        <v>3.3125000000002176E-3</v>
+      </c>
       <c r="W59" t="s">
         <v>376</v>
       </c>
@@ -8254,7 +8496,7 @@
         <v>3.6999999999999998E-2</v>
       </c>
       <c r="O60" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>278203000</v>
       </c>
       <c r="Q60" t="s">
@@ -8273,6 +8515,10 @@
         <f t="shared" si="1"/>
         <v>#VALUE!</v>
       </c>
+      <c r="V60" s="1" t="e">
+        <f t="shared" si="2"/>
+        <v>#VALUE!</v>
+      </c>
       <c r="W60" t="s">
         <v>377</v>
       </c>
@@ -8324,7 +8570,7 @@
         <v>0.39</v>
       </c>
       <c r="I61" s="1">
-        <f t="shared" ref="I61:I82" si="5">G61/1000000*37000000000*H61</f>
+        <f t="shared" ref="I61:I82" si="6">G61/1000000*37000000000*H61</f>
         <v>438354540</v>
       </c>
       <c r="K61" t="s">
@@ -8340,7 +8586,7 @@
         <v>0.39</v>
       </c>
       <c r="O61" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>391560000</v>
       </c>
       <c r="Q61" t="s">
@@ -8359,6 +8605,10 @@
         <f t="shared" si="1"/>
         <v>436800000</v>
       </c>
+      <c r="V61" s="1">
+        <f t="shared" si="2"/>
+        <v>3.5589285714285714E-3</v>
+      </c>
       <c r="W61" t="s">
         <v>378</v>
       </c>
@@ -8410,7 +8660,7 @@
         <v>0.746</v>
       </c>
       <c r="I62" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>12897034500</v>
       </c>
       <c r="K62" t="s">
@@ -8426,7 +8676,7 @@
         <v>0.746</v>
       </c>
       <c r="O62" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>20425480000</v>
       </c>
       <c r="Q62" t="s">
@@ -8445,6 +8695,10 @@
         <f t="shared" si="1"/>
         <v>13037500000</v>
       </c>
+      <c r="V62" s="1">
+        <f t="shared" si="2"/>
+        <v>1.0773959731543624E-2</v>
+      </c>
       <c r="W62" t="s">
         <v>379</v>
       </c>
@@ -8496,7 +8750,7 @@
         <v>0.14199999999999999</v>
       </c>
       <c r="I63" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>268637019999.99997</v>
       </c>
       <c r="K63" s="4" t="s">
@@ -8512,7 +8766,7 @@
         <v>0.2853</v>
       </c>
       <c r="O63" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>126815850</v>
       </c>
       <c r="Q63" t="s">
@@ -8531,6 +8785,10 @@
         <f t="shared" si="1"/>
         <v>268379999999.99997</v>
       </c>
+      <c r="V63" s="1">
+        <f t="shared" si="2"/>
+        <v>9.5767195767195779E-4</v>
+      </c>
       <c r="W63" t="s">
         <v>380</v>
       </c>
@@ -8582,7 +8840,7 @@
         <v>0.60099999999999998</v>
       </c>
       <c r="I64" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1640423490</v>
       </c>
       <c r="K64" s="4" t="s">
@@ -8598,7 +8856,7 @@
         <v>0.1178</v>
       </c>
       <c r="O64" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>38791540000</v>
       </c>
       <c r="Q64" t="s">
@@ -8617,6 +8875,10 @@
         <f t="shared" si="1"/>
         <v>1634720000</v>
       </c>
+      <c r="V64" s="1">
+        <f t="shared" si="2"/>
+        <v>3.4889705882352943E-3</v>
+      </c>
       <c r="W64" t="s">
         <v>381</v>
       </c>
@@ -8668,7 +8930,7 @@
         <v>0.30099999999999999</v>
       </c>
       <c r="I65" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>45553671.100000001</v>
       </c>
       <c r="K65" t="s">
@@ -8684,7 +8946,7 @@
         <v>0.30099999999999999</v>
       </c>
       <c r="O65" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>45631600</v>
       </c>
       <c r="Q65" t="s">
@@ -8703,6 +8965,10 @@
         <f t="shared" si="1"/>
         <v>45451000</v>
       </c>
+      <c r="V65" s="1">
+        <f t="shared" si="2"/>
+        <v>2.2589403973510263E-3</v>
+      </c>
       <c r="W65" t="s">
         <v>382</v>
       </c>
@@ -8754,7 +9020,7 @@
         <v>3.0099999999999998E-2</v>
       </c>
       <c r="I66" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>227707102000</v>
       </c>
       <c r="K66" s="4" t="s">
@@ -8770,7 +9036,7 @@
         <v>3.7999999999999999E-2</v>
       </c>
       <c r="O66" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>115862000000</v>
       </c>
       <c r="Q66" t="s">
@@ -8789,6 +9055,10 @@
         <f t="shared" si="1"/>
         <v>227556000000</v>
       </c>
+      <c r="V66" s="1">
+        <f t="shared" si="2"/>
+        <v>6.6402116402116405E-4</v>
+      </c>
       <c r="W66" t="s">
         <v>383</v>
       </c>
@@ -8840,7 +9110,7 @@
         <v>6.7100000000000007E-2</v>
       </c>
       <c r="I67" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1621798948.0000002</v>
       </c>
       <c r="K67" t="s">
@@ -8856,7 +9126,7 @@
         <v>6.7100000000000007E-2</v>
       </c>
       <c r="O67" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1739903000.0000002</v>
       </c>
       <c r="Q67" t="s">
@@ -8875,6 +9145,10 @@
         <f t="shared" si="1"/>
         <v>1587520000.0000002</v>
       </c>
+      <c r="V67" s="1">
+        <f t="shared" si="2"/>
+        <v>2.1592766075388025E-2</v>
+      </c>
       <c r="W67" t="s">
         <v>384</v>
       </c>
@@ -8926,7 +9200,7 @@
         <v>0.41699999999999998</v>
       </c>
       <c r="I68" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>32603019900</v>
       </c>
       <c r="K68" s="4" t="s">
@@ -8942,7 +9216,7 @@
         <v>0.64</v>
       </c>
       <c r="O68" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1150080000</v>
       </c>
       <c r="Q68" t="s">
@@ -8961,6 +9235,10 @@
         <f t="shared" si="1"/>
         <v>33368800000</v>
       </c>
+      <c r="V68" s="1">
+        <f t="shared" si="2"/>
+        <v>2.2948985279662441E-2</v>
+      </c>
       <c r="W68" t="s">
         <v>385</v>
       </c>
@@ -9012,7 +9290,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="I69" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>8765670</v>
       </c>
       <c r="K69" t="s">
@@ -9028,7 +9306,7 @@
         <v>2.5000000000000001E-2</v>
       </c>
       <c r="O69" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>9035000000</v>
       </c>
       <c r="Q69" t="s">
@@ -9047,6 +9325,10 @@
         <f t="shared" si="1"/>
         <v>8704800</v>
       </c>
+      <c r="V69" s="1">
+        <f t="shared" si="2"/>
+        <v>6.9926936862420731E-3</v>
+      </c>
       <c r="W69" t="s">
         <v>386</v>
       </c>
@@ -9114,7 +9396,7 @@
         <v>0.13200000000000001</v>
       </c>
       <c r="O70" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>272712000</v>
       </c>
       <c r="Q70" t="s">
@@ -9130,8 +9412,12 @@
         <v>3.8800000000000001E-6</v>
       </c>
       <c r="U70" s="1">
-        <f t="shared" si="1"/>
+        <f>S70*T70</f>
         <v>269660</v>
+      </c>
+      <c r="V70" s="1">
+        <f t="shared" si="2"/>
+        <v>613584.32744938065</v>
       </c>
       <c r="W70" s="4" t="s">
         <v>387</v>
@@ -9184,7 +9470,7 @@
         <v>8.8999999999999996E-2</v>
       </c>
       <c r="I71" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>3317368200</v>
       </c>
       <c r="K71" s="4" t="s">
@@ -9200,7 +9486,7 @@
         <v>0.1041</v>
       </c>
       <c r="O71" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>360914700</v>
       </c>
       <c r="Q71" t="s">
@@ -9219,6 +9505,10 @@
         <f t="shared" si="1"/>
         <v>3319700000</v>
       </c>
+      <c r="V71" s="1">
+        <f t="shared" si="2"/>
+        <v>7.0241286863270778E-4</v>
+      </c>
       <c r="W71" t="s">
         <v>388</v>
       </c>
@@ -9270,7 +9560,7 @@
         <v>0.94</v>
       </c>
       <c r="I72" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>196437440000</v>
       </c>
       <c r="K72" s="4" t="s">
@@ -9286,7 +9576,7 @@
         <v>0.80500000000000005</v>
       </c>
       <c r="O72" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>36506750</v>
       </c>
       <c r="Q72" t="s">
@@ -9305,6 +9595,10 @@
         <f t="shared" si="1"/>
         <v>200130000000</v>
       </c>
+      <c r="V72" s="1">
+        <f t="shared" si="2"/>
+        <v>1.8450806975465948E-2</v>
+      </c>
       <c r="W72" t="s">
         <v>389</v>
       </c>
@@ -9356,7 +9650,7 @@
         <v>0.49</v>
       </c>
       <c r="I73" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>77358897</v>
       </c>
       <c r="K73" t="s">
@@ -9372,7 +9666,7 @@
         <v>0.41199999999999998</v>
       </c>
       <c r="O73" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>30352040</v>
       </c>
       <c r="Q73" t="s">
@@ -9391,6 +9685,10 @@
         <f t="shared" si="1"/>
         <v>75840000</v>
       </c>
+      <c r="V73" s="1">
+        <f t="shared" si="2"/>
+        <v>2.0027650316455696E-2</v>
+      </c>
       <c r="W73" t="s">
         <v>390</v>
       </c>
@@ -9442,7 +9740,7 @@
         <v>0.27300000000000002</v>
       </c>
       <c r="I74" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1141817040</v>
       </c>
       <c r="K74" t="s">
@@ -9458,7 +9756,7 @@
         <v>0.27300000000000002</v>
       </c>
       <c r="O74" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>1210482000</v>
       </c>
       <c r="Q74" t="s">
@@ -9477,6 +9775,10 @@
         <f t="shared" si="1"/>
         <v>1391080000</v>
       </c>
+      <c r="V74" s="1">
+        <f t="shared" si="2"/>
+        <v>0.1791866463467234</v>
+      </c>
       <c r="W74" t="s">
         <v>391</v>
       </c>
@@ -9528,7 +9830,7 @@
         <v>0.216</v>
       </c>
       <c r="I75" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>122557320000</v>
       </c>
       <c r="K75" s="4" t="s">
@@ -9544,7 +9846,7 @@
         <v>0.15490000000000001</v>
       </c>
       <c r="O75" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4121889000.0000005</v>
       </c>
       <c r="Q75" t="s">
@@ -9560,8 +9862,12 @@
         <v>0.223</v>
       </c>
       <c r="U75" s="1">
-        <f t="shared" ref="U75:U85" si="6">S75*T75</f>
+        <f t="shared" ref="U75:U85" si="7">S75*T75</f>
         <v>125772000000</v>
+      </c>
+      <c r="V75" s="1">
+        <f t="shared" ref="V75:V85" si="8">ABS(I75-U75)/U75</f>
+        <v>2.555958400915943E-2</v>
       </c>
       <c r="W75" t="s">
         <v>392</v>
@@ -9614,7 +9920,7 @@
         <v>6.9999999999999999E-4</v>
       </c>
       <c r="I76" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>1501526.6</v>
       </c>
       <c r="K76" t="s">
@@ -9630,7 +9936,7 @@
         <v>4.2700000000000002E-2</v>
       </c>
       <c r="O76" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>16986060</v>
       </c>
       <c r="Q76" t="s">
@@ -9646,7 +9952,11 @@
         <v>403</v>
       </c>
       <c r="U76" s="1" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V76" s="1" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="W76" t="s">
@@ -9701,7 +10011,7 @@
         <v>3.3993880000000003E-4</v>
       </c>
       <c r="I77" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>532377814.74120003</v>
       </c>
       <c r="K77" t="s">
@@ -9717,7 +10027,7 @@
         <v>0.13100000000000001</v>
       </c>
       <c r="O77" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>4366230000</v>
       </c>
       <c r="Q77" t="s">
@@ -9733,8 +10043,12 @@
         <v>3.5070000000000001E-4</v>
       </c>
       <c r="U77" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>533064000</v>
+      </c>
+      <c r="V77" s="1">
+        <f t="shared" si="8"/>
+        <v>1.2872474201971436E-3</v>
       </c>
       <c r="W77" t="s">
         <v>394</v>
@@ -9787,7 +10101,7 @@
         <v>0.15</v>
       </c>
       <c r="I78" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>385491900</v>
       </c>
       <c r="K78" t="s">
@@ -9803,7 +10117,7 @@
         <v>0.15</v>
       </c>
       <c r="O78" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>388800000</v>
       </c>
       <c r="Q78" t="s">
@@ -9819,8 +10133,12 @@
         <v>0.1174</v>
       </c>
       <c r="U78" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>300544000</v>
+      </c>
+      <c r="V78" s="1">
+        <f t="shared" si="8"/>
+        <v>0.28264713319846679</v>
       </c>
       <c r="W78" t="s">
         <v>395</v>
@@ -9873,7 +10191,7 @@
         <v>0.96</v>
       </c>
       <c r="I79" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>13263878399.999998</v>
       </c>
       <c r="K79" t="s">
@@ -9889,7 +10207,7 @@
         <v>0.96</v>
       </c>
       <c r="O79" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>13267200000</v>
       </c>
       <c r="Q79" t="s">
@@ -9905,8 +10223,12 @@
         <v>0.95620000000000005</v>
       </c>
       <c r="U79" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>13195560000</v>
+      </c>
+      <c r="V79" s="1">
+        <f t="shared" si="8"/>
+        <v>5.1773778452750847E-3</v>
       </c>
       <c r="W79" t="s">
         <v>396</v>
@@ -9959,7 +10281,7 @@
         <v>0.187</v>
       </c>
       <c r="I80" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>117858246</v>
       </c>
       <c r="K80" t="s">
@@ -9975,7 +10297,7 @@
         <v>0.187</v>
       </c>
       <c r="O80" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>159978500</v>
       </c>
       <c r="Q80" t="s">
@@ -9991,7 +10313,11 @@
         <v>403</v>
       </c>
       <c r="U80" s="1" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V80" s="1" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="W80" t="s">
@@ -10045,7 +10371,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="I81" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>44529.5</v>
       </c>
       <c r="K81" t="s">
@@ -10061,7 +10387,7 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="O81" s="1">
-        <f t="shared" si="4"/>
+        <f t="shared" si="5"/>
         <v>46445</v>
       </c>
       <c r="Q81" t="s">
@@ -10077,8 +10403,12 @@
         <v>5.0000000000000002E-5</v>
       </c>
       <c r="U81" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>44500</v>
+      </c>
+      <c r="V81" s="1">
+        <f t="shared" si="8"/>
+        <v>6.6292134831460678E-4</v>
       </c>
       <c r="W81" t="s">
         <v>398</v>
@@ -10116,7 +10446,7 @@
         <v>16238</v>
       </c>
       <c r="I82" s="1">
-        <f t="shared" si="5"/>
+        <f t="shared" si="6"/>
         <v>0</v>
       </c>
       <c r="K82" t="s">
@@ -10142,7 +10472,11 @@
         <v>403</v>
       </c>
       <c r="U82" s="1" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V82" s="1" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="AC82" s="21" t="s">
@@ -10207,7 +10541,11 @@
         <v>403</v>
       </c>
       <c r="U83" s="1" t="e">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
+        <v>#VALUE!</v>
+      </c>
+      <c r="V83" s="1" t="e">
+        <f t="shared" si="8"/>
         <v>#VALUE!</v>
       </c>
       <c r="W83" s="4" t="s">
@@ -10269,8 +10607,12 @@
       <c r="S84" s="13"/>
       <c r="T84" s="12"/>
       <c r="U84" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
+      </c>
+      <c r="V84" s="1" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="W84" t="s">
         <v>400</v>
@@ -10331,8 +10673,12 @@
       <c r="S85" s="13"/>
       <c r="T85" s="12"/>
       <c r="U85" s="1">
-        <f t="shared" si="6"/>
+        <f t="shared" si="7"/>
         <v>0</v>
+      </c>
+      <c r="V85" s="1" t="e">
+        <f t="shared" si="8"/>
+        <v>#DIV/0!</v>
       </c>
       <c r="W85" t="s">
         <v>401</v>
@@ -10352,6 +10698,18 @@
     </row>
   </sheetData>
   <phoneticPr fontId="18" type="noConversion"/>
+  <conditionalFormatting sqref="V10:V85">
+    <cfRule type="colorScale" priority="1">
+      <colorScale>
+        <cfvo type="min"/>
+        <cfvo type="percentile" val="50"/>
+        <cfvo type="max"/>
+        <color rgb="FFF8696B"/>
+        <color rgb="FFFFEB84"/>
+        <color rgb="FF63BE7B"/>
+      </colorScale>
+    </cfRule>
+  </conditionalFormatting>
   <hyperlinks>
     <hyperlink ref="E3" r:id="rId1" xr:uid="{08D4AC46-BB46-4859-B631-4043224F8795}"/>
     <hyperlink ref="K3" r:id="rId2" xr:uid="{A7517F8A-2B7B-4E37-BE20-6AFA39231E2E}"/>
@@ -10365,11 +10723,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8A9232AB-CB9F-47AD-BB52-A50DAE889965}">
   <dimension ref="A1:H75"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+    <sheetView zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B51" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
-      <selection pane="bottomRight" activeCell="E3" sqref="E3"/>
+      <selection pane="bottomRight" activeCell="D75" sqref="D75"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -11593,13 +11951,13 @@
         <v>753</v>
       </c>
       <c r="D55" s="18" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="E55" s="18" t="s">
         <v>753</v>
       </c>
       <c r="F55" s="18" t="s">
-        <v>753</v>
+        <v>757</v>
       </c>
       <c r="H55">
         <v>62</v>
@@ -11754,13 +12112,13 @@
         <v>754</v>
       </c>
       <c r="D62" s="18" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
       <c r="E62" s="18" t="s">
         <v>754</v>
       </c>
       <c r="F62" s="18" t="s">
-        <v>754</v>
+        <v>759</v>
       </c>
       <c r="H62">
         <v>69</v>
@@ -12073,7 +12431,7 @@
   <dimension ref="A1:K39"/>
   <sheetViews>
     <sheetView zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="1" ySplit="2" topLeftCell="B12" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="E1" sqref="E1"/>
       <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
       <selection pane="bottomRight" activeCell="G26" sqref="G26"/>
@@ -13330,4 +13688,1609 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{11CF74B6-4303-47C6-A56C-3276C56A21E4}">
+  <dimension ref="A1:P75"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
+      <pane xSplit="1" ySplit="2" topLeftCell="B3" activePane="bottomRight" state="frozen"/>
+      <selection pane="topRight" activeCell="E1" sqref="E1"/>
+      <selection pane="bottomLeft" activeCell="A10" sqref="A10"/>
+      <selection pane="bottomRight" activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="6" width="8.33203125" customWidth="1"/>
+    <col min="7" max="7" width="4.77734375" customWidth="1"/>
+    <col min="8" max="12" width="8.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:16" ht="14.4" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="A1" s="58" t="s">
+        <v>614</v>
+      </c>
+      <c r="B1" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="C1" s="58"/>
+      <c r="D1" s="58"/>
+      <c r="E1" s="58"/>
+      <c r="F1" s="58"/>
+      <c r="G1" s="41"/>
+      <c r="H1" s="58" t="s">
+        <v>614</v>
+      </c>
+      <c r="I1" s="58" t="s">
+        <v>226</v>
+      </c>
+      <c r="J1" s="58"/>
+      <c r="K1" s="58"/>
+      <c r="L1" s="58"/>
+      <c r="M1" s="58"/>
+      <c r="N1" s="62"/>
+      <c r="O1" s="62"/>
+      <c r="P1" s="62"/>
+    </row>
+    <row r="2" spans="1:16" s="2" customFormat="1" x14ac:dyDescent="0.25">
+      <c r="A2" s="60"/>
+      <c r="B2" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="C2" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="D2" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="E2" s="28" t="s">
+        <v>612</v>
+      </c>
+      <c r="F2" s="28" t="s">
+        <v>615</v>
+      </c>
+      <c r="G2" s="28"/>
+      <c r="H2" s="59"/>
+      <c r="I2" s="28" t="s">
+        <v>523</v>
+      </c>
+      <c r="J2" s="28" t="s">
+        <v>326</v>
+      </c>
+      <c r="K2" s="28" t="s">
+        <v>613</v>
+      </c>
+      <c r="L2" s="28" t="s">
+        <v>612</v>
+      </c>
+      <c r="M2" s="28" t="s">
+        <v>615</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A3" s="27" t="s">
+        <v>11</v>
+      </c>
+      <c r="B3" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="C3" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="D3" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="E3" s="27" t="s">
+        <v>328</v>
+      </c>
+      <c r="F3" s="18" t="s">
+        <v>328</v>
+      </c>
+      <c r="G3" s="18"/>
+      <c r="H3" s="27" t="s">
+        <v>110</v>
+      </c>
+      <c r="I3" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="J3" s="33" t="s">
+        <v>364</v>
+      </c>
+      <c r="K3" s="27" t="s">
+        <v>567</v>
+      </c>
+      <c r="L3" s="27" t="s">
+        <v>567</v>
+      </c>
+      <c r="M3" s="18" t="s">
+        <v>567</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A4" s="27" t="s">
+        <v>14</v>
+      </c>
+      <c r="B4" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="C4" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="D4" s="27" t="s">
+        <v>329</v>
+      </c>
+      <c r="E4" s="27"/>
+      <c r="F4" s="18" t="s">
+        <v>329</v>
+      </c>
+      <c r="G4" s="18"/>
+      <c r="H4" s="27" t="s">
+        <v>113</v>
+      </c>
+      <c r="I4" s="27" t="s">
+        <v>365</v>
+      </c>
+      <c r="J4" s="27" t="s">
+        <v>365</v>
+      </c>
+      <c r="K4" s="29" t="s">
+        <v>365</v>
+      </c>
+      <c r="L4" s="27" t="s">
+        <v>365</v>
+      </c>
+      <c r="M4" s="18" t="s">
+        <v>365</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="B5" s="27"/>
+      <c r="C5" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="D5" s="27" t="s">
+        <v>330</v>
+      </c>
+      <c r="E5" s="27"/>
+      <c r="F5" s="18" t="s">
+        <v>330</v>
+      </c>
+      <c r="G5" s="18"/>
+      <c r="H5" s="27" t="s">
+        <v>114</v>
+      </c>
+      <c r="I5" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="J5" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="K5" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="L5" s="30" t="s">
+        <v>568</v>
+      </c>
+      <c r="M5" s="18" t="s">
+        <v>366</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A6" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="B6" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="C6" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="D6" s="61" t="s">
+        <v>331</v>
+      </c>
+      <c r="E6" s="27" t="s">
+        <v>331</v>
+      </c>
+      <c r="F6" s="18" t="s">
+        <v>331</v>
+      </c>
+      <c r="G6" s="18"/>
+      <c r="H6" s="27" t="s">
+        <v>117</v>
+      </c>
+      <c r="I6" s="27" t="s">
+        <v>367</v>
+      </c>
+      <c r="J6" s="27" t="s">
+        <v>367</v>
+      </c>
+      <c r="K6" s="29" t="s">
+        <v>596</v>
+      </c>
+      <c r="L6" s="30" t="s">
+        <v>569</v>
+      </c>
+      <c r="M6" s="18" t="s">
+        <v>596</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A7" s="27" t="s">
+        <v>19</v>
+      </c>
+      <c r="B7" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="C7" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="D7" s="27" t="s">
+        <v>332</v>
+      </c>
+      <c r="E7" s="27"/>
+      <c r="F7" s="18" t="s">
+        <v>332</v>
+      </c>
+      <c r="G7" s="18"/>
+      <c r="H7" s="27" t="s">
+        <v>120</v>
+      </c>
+      <c r="I7" s="30" t="s">
+        <v>571</v>
+      </c>
+      <c r="J7" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="K7" s="27" t="s">
+        <v>368</v>
+      </c>
+      <c r="L7" s="30" t="s">
+        <v>570</v>
+      </c>
+      <c r="M7" s="25" t="s">
+        <v>740</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A8" s="27" t="s">
+        <v>20</v>
+      </c>
+      <c r="B8" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="C8" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="D8" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="E8" s="27" t="s">
+        <v>333</v>
+      </c>
+      <c r="F8" s="18" t="s">
+        <v>333</v>
+      </c>
+      <c r="G8" s="18"/>
+      <c r="H8" s="27" t="s">
+        <v>123</v>
+      </c>
+      <c r="I8" s="27" t="s">
+        <v>572</v>
+      </c>
+      <c r="J8" s="30" t="s">
+        <v>369</v>
+      </c>
+      <c r="K8" s="27" t="s">
+        <v>572</v>
+      </c>
+      <c r="L8" s="27" t="s">
+        <v>572</v>
+      </c>
+      <c r="M8" s="18" t="s">
+        <v>572</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A9" s="27" t="s">
+        <v>23</v>
+      </c>
+      <c r="B9" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="C9" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="D9" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="E9" s="27" t="s">
+        <v>334</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>334</v>
+      </c>
+      <c r="G9" s="18"/>
+      <c r="H9" s="27" t="s">
+        <v>126</v>
+      </c>
+      <c r="I9" s="27" t="s">
+        <v>370</v>
+      </c>
+      <c r="J9" s="27" t="s">
+        <v>370</v>
+      </c>
+      <c r="K9" s="27" t="s">
+        <v>573</v>
+      </c>
+      <c r="L9" s="27" t="s">
+        <v>370</v>
+      </c>
+      <c r="M9" s="18" t="s">
+        <v>748</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A10" s="27" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="27"/>
+      <c r="C10" s="27"/>
+      <c r="D10" s="27" t="s">
+        <v>548</v>
+      </c>
+      <c r="E10" s="27" t="s">
+        <v>548</v>
+      </c>
+      <c r="F10" s="18" t="s">
+        <v>548</v>
+      </c>
+      <c r="G10" s="18"/>
+      <c r="H10" s="27" t="s">
+        <v>129</v>
+      </c>
+      <c r="I10" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="J10" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="K10" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="L10" s="27" t="s">
+        <v>371</v>
+      </c>
+      <c r="M10" s="18" t="s">
+        <v>371</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A11" s="27" t="s">
+        <v>29</v>
+      </c>
+      <c r="B11" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>335</v>
+      </c>
+      <c r="E11" s="30" t="s">
+        <v>549</v>
+      </c>
+      <c r="F11" s="18" t="s">
+        <v>549</v>
+      </c>
+      <c r="G11" s="18"/>
+      <c r="H11" s="27" t="s">
+        <v>132</v>
+      </c>
+      <c r="I11" s="27"/>
+      <c r="J11" s="32" t="s">
+        <v>372</v>
+      </c>
+      <c r="K11" s="32" t="s">
+        <v>597</v>
+      </c>
+      <c r="L11" s="32" t="s">
+        <v>574</v>
+      </c>
+      <c r="M11" s="26" t="s">
+        <v>741</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A12" s="27" t="s">
+        <v>32</v>
+      </c>
+      <c r="B12" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="C12" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="D12" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="E12" s="27" t="s">
+        <v>336</v>
+      </c>
+      <c r="F12" s="18" t="s">
+        <v>336</v>
+      </c>
+      <c r="G12" s="18"/>
+      <c r="H12" s="27" t="s">
+        <v>135</v>
+      </c>
+      <c r="I12" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="J12" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="K12" s="27" t="s">
+        <v>598</v>
+      </c>
+      <c r="L12" s="30" t="s">
+        <v>575</v>
+      </c>
+      <c r="M12" s="18" t="s">
+        <v>373</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A13" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="B13" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="C13" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="D13" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="E13" s="27" t="s">
+        <v>337</v>
+      </c>
+      <c r="F13" s="18" t="s">
+        <v>337</v>
+      </c>
+      <c r="G13" s="18"/>
+      <c r="H13" s="27" t="s">
+        <v>138</v>
+      </c>
+      <c r="I13" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="J13" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="K13" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="L13" s="27" t="s">
+        <v>374</v>
+      </c>
+      <c r="M13" s="18" t="s">
+        <v>374</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A14" s="27" t="s">
+        <v>38</v>
+      </c>
+      <c r="B14" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="C14" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="D14" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="E14" s="27" t="s">
+        <v>338</v>
+      </c>
+      <c r="F14" s="18" t="s">
+        <v>338</v>
+      </c>
+      <c r="G14" s="18"/>
+      <c r="H14" s="27" t="s">
+        <v>141</v>
+      </c>
+      <c r="I14" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="J14" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="K14" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="L14" s="27" t="s">
+        <v>375</v>
+      </c>
+      <c r="M14" s="18" t="s">
+        <v>375</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A15" s="27" t="s">
+        <v>41</v>
+      </c>
+      <c r="B15" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="C15" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="D15" s="27" t="s">
+        <v>339</v>
+      </c>
+      <c r="E15" s="27" t="s">
+        <v>611</v>
+      </c>
+      <c r="F15" s="18" t="s">
+        <v>611</v>
+      </c>
+      <c r="G15" s="18"/>
+      <c r="H15" s="27" t="s">
+        <v>144</v>
+      </c>
+      <c r="I15" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="J15" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="K15" s="27" t="s">
+        <v>599</v>
+      </c>
+      <c r="L15" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="M15" s="18" t="s">
+        <v>599</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="A16" s="27" t="s">
+        <v>44</v>
+      </c>
+      <c r="B16" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="C16" s="27" t="s">
+        <v>340</v>
+      </c>
+      <c r="D16" s="27" t="s">
+        <v>591</v>
+      </c>
+      <c r="E16" s="30" t="s">
+        <v>550</v>
+      </c>
+      <c r="F16" s="18" t="s">
+        <v>340</v>
+      </c>
+      <c r="G16" s="18"/>
+      <c r="H16" s="27" t="s">
+        <v>147</v>
+      </c>
+      <c r="I16" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="J16" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="K16" s="30" t="s">
+        <v>600</v>
+      </c>
+      <c r="L16" s="27" t="s">
+        <v>377</v>
+      </c>
+      <c r="M16" s="25" t="s">
+        <v>742</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A17" s="27" t="s">
+        <v>47</v>
+      </c>
+      <c r="B17" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="C17" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="D17" s="27" t="s">
+        <v>341</v>
+      </c>
+      <c r="E17" s="28"/>
+      <c r="F17" s="18" t="s">
+        <v>341</v>
+      </c>
+      <c r="G17" s="18"/>
+      <c r="H17" s="27" t="s">
+        <v>150</v>
+      </c>
+      <c r="I17" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="J17" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="K17" s="27" t="s">
+        <v>601</v>
+      </c>
+      <c r="L17" s="27" t="s">
+        <v>378</v>
+      </c>
+      <c r="M17" s="18" t="s">
+        <v>601</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A18" s="27" t="s">
+        <v>48</v>
+      </c>
+      <c r="B18" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="C18" s="27" t="s">
+        <v>342</v>
+      </c>
+      <c r="D18" s="29" t="s">
+        <v>342</v>
+      </c>
+      <c r="E18" s="28"/>
+      <c r="F18" s="18" t="s">
+        <v>342</v>
+      </c>
+      <c r="G18" s="18"/>
+      <c r="H18" s="27" t="s">
+        <v>153</v>
+      </c>
+      <c r="I18" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="J18" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="K18" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="L18" s="27" t="s">
+        <v>379</v>
+      </c>
+      <c r="M18" s="18" t="s">
+        <v>756</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A19" s="27" t="s">
+        <v>49</v>
+      </c>
+      <c r="B19" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="C19" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="D19" s="30" t="s">
+        <v>551</v>
+      </c>
+      <c r="E19" s="27" t="s">
+        <v>343</v>
+      </c>
+      <c r="F19" s="25" t="s">
+        <v>551</v>
+      </c>
+      <c r="G19" s="18"/>
+      <c r="H19" s="27" t="s">
+        <v>156</v>
+      </c>
+      <c r="I19" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="J19" s="27" t="s">
+        <v>380</v>
+      </c>
+      <c r="K19" s="29" t="s">
+        <v>602</v>
+      </c>
+      <c r="L19" s="30" t="s">
+        <v>576</v>
+      </c>
+      <c r="M19" s="18" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A20" s="27" t="s">
+        <v>52</v>
+      </c>
+      <c r="B20" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="C20" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="D20" s="29" t="s">
+        <v>344</v>
+      </c>
+      <c r="E20" s="27" t="s">
+        <v>344</v>
+      </c>
+      <c r="F20" s="18" t="s">
+        <v>344</v>
+      </c>
+      <c r="G20" s="18"/>
+      <c r="H20" s="27" t="s">
+        <v>159</v>
+      </c>
+      <c r="I20" s="33" t="s">
+        <v>577</v>
+      </c>
+      <c r="J20" s="27" t="s">
+        <v>381</v>
+      </c>
+      <c r="K20" s="27" t="s">
+        <v>603</v>
+      </c>
+      <c r="L20" s="33" t="s">
+        <v>577</v>
+      </c>
+      <c r="M20" s="18" t="s">
+        <v>603</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A21" s="27" t="s">
+        <v>55</v>
+      </c>
+      <c r="B21" s="27" t="s">
+        <v>345</v>
+      </c>
+      <c r="C21" s="30" t="s">
+        <v>345</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>552</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>552</v>
+      </c>
+      <c r="F21" s="18" t="s">
+        <v>552</v>
+      </c>
+      <c r="G21" s="18"/>
+      <c r="H21" s="27" t="s">
+        <v>162</v>
+      </c>
+      <c r="I21" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="J21" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="K21" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="L21" s="27" t="s">
+        <v>382</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>382</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A22" s="27" t="s">
+        <v>58</v>
+      </c>
+      <c r="B22" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>346</v>
+      </c>
+      <c r="D22" s="29" t="s">
+        <v>592</v>
+      </c>
+      <c r="E22" s="30" t="s">
+        <v>553</v>
+      </c>
+      <c r="F22" s="18" t="s">
+        <v>346</v>
+      </c>
+      <c r="G22" s="18"/>
+      <c r="H22" s="27" t="s">
+        <v>165</v>
+      </c>
+      <c r="I22" s="27" t="s">
+        <v>383</v>
+      </c>
+      <c r="J22" s="27" t="s">
+        <v>383</v>
+      </c>
+      <c r="K22" s="29" t="s">
+        <v>383</v>
+      </c>
+      <c r="L22" s="30" t="s">
+        <v>578</v>
+      </c>
+      <c r="M22" s="18" t="s">
+        <v>383</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A23" s="27" t="s">
+        <v>61</v>
+      </c>
+      <c r="B23" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="C23" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="D23" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="E23" s="27" t="s">
+        <v>347</v>
+      </c>
+      <c r="F23" s="18" t="s">
+        <v>347</v>
+      </c>
+      <c r="G23" s="18"/>
+      <c r="H23" s="27" t="s">
+        <v>168</v>
+      </c>
+      <c r="I23" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="J23" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="K23" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="L23" s="27" t="s">
+        <v>384</v>
+      </c>
+      <c r="M23" s="18" t="s">
+        <v>384</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A24" s="27" t="s">
+        <v>64</v>
+      </c>
+      <c r="B24" s="30" t="s">
+        <v>554</v>
+      </c>
+      <c r="C24" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="D24" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="E24" s="27" t="s">
+        <v>348</v>
+      </c>
+      <c r="F24" s="18" t="s">
+        <v>348</v>
+      </c>
+      <c r="G24" s="18"/>
+      <c r="H24" s="27" t="s">
+        <v>171</v>
+      </c>
+      <c r="I24" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="J24" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="K24" s="27" t="s">
+        <v>385</v>
+      </c>
+      <c r="L24" s="30" t="s">
+        <v>579</v>
+      </c>
+      <c r="M24" s="18" t="s">
+        <v>385</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A25" s="27" t="s">
+        <v>67</v>
+      </c>
+      <c r="B25" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="C25" s="33" t="s">
+        <v>349</v>
+      </c>
+      <c r="D25" s="27" t="s">
+        <v>555</v>
+      </c>
+      <c r="E25" s="27" t="s">
+        <v>555</v>
+      </c>
+      <c r="F25" s="18" t="s">
+        <v>555</v>
+      </c>
+      <c r="G25" s="18"/>
+      <c r="H25" s="27" t="s">
+        <v>174</v>
+      </c>
+      <c r="I25" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="J25" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="K25" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="L25" s="27" t="s">
+        <v>386</v>
+      </c>
+      <c r="M25" s="18" t="s">
+        <v>758</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A26" s="27" t="s">
+        <v>70</v>
+      </c>
+      <c r="B26" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="C26" s="33" t="s">
+        <v>350</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>556</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>556</v>
+      </c>
+      <c r="F26" s="18" t="s">
+        <v>556</v>
+      </c>
+      <c r="G26" s="18"/>
+      <c r="H26" s="27" t="s">
+        <v>177</v>
+      </c>
+      <c r="I26" s="32" t="s">
+        <v>581</v>
+      </c>
+      <c r="J26" s="32" t="s">
+        <v>387</v>
+      </c>
+      <c r="K26" s="34" t="s">
+        <v>604</v>
+      </c>
+      <c r="L26" s="32" t="s">
+        <v>580</v>
+      </c>
+      <c r="M26" s="34" t="s">
+        <v>604</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A27" s="27" t="s">
+        <v>73</v>
+      </c>
+      <c r="B27" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="C27" s="33" t="s">
+        <v>351</v>
+      </c>
+      <c r="D27" s="63" t="s">
+        <v>557</v>
+      </c>
+      <c r="E27" s="27" t="s">
+        <v>557</v>
+      </c>
+      <c r="F27" s="18" t="s">
+        <v>557</v>
+      </c>
+      <c r="G27" s="18"/>
+      <c r="H27" s="27" t="s">
+        <v>180</v>
+      </c>
+      <c r="I27" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="J27" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="K27" s="27" t="s">
+        <v>388</v>
+      </c>
+      <c r="L27" s="30" t="s">
+        <v>582</v>
+      </c>
+      <c r="M27" s="18" t="s">
+        <v>388</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A28" s="27" t="s">
+        <v>76</v>
+      </c>
+      <c r="B28" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="C28" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="D28" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="E28" s="27" t="s">
+        <v>352</v>
+      </c>
+      <c r="F28" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="G28" s="18"/>
+      <c r="H28" s="27" t="s">
+        <v>183</v>
+      </c>
+      <c r="I28" s="27" t="s">
+        <v>389</v>
+      </c>
+      <c r="J28" s="27" t="s">
+        <v>389</v>
+      </c>
+      <c r="K28" s="27" t="s">
+        <v>605</v>
+      </c>
+      <c r="L28" s="30" t="s">
+        <v>583</v>
+      </c>
+      <c r="M28" s="18" t="s">
+        <v>389</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A29" s="27" t="s">
+        <v>79</v>
+      </c>
+      <c r="B29" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="C29" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="D29" s="27" t="s">
+        <v>353</v>
+      </c>
+      <c r="E29" s="30" t="s">
+        <v>558</v>
+      </c>
+      <c r="F29" s="18" t="s">
+        <v>353</v>
+      </c>
+      <c r="G29" s="18"/>
+      <c r="H29" s="27" t="s">
+        <v>186</v>
+      </c>
+      <c r="I29" s="33" t="s">
+        <v>584</v>
+      </c>
+      <c r="J29" s="27" t="s">
+        <v>390</v>
+      </c>
+      <c r="K29" s="33" t="s">
+        <v>606</v>
+      </c>
+      <c r="L29" s="27" t="s">
+        <v>390</v>
+      </c>
+      <c r="M29" s="33" t="s">
+        <v>606</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A30" s="27" t="s">
+        <v>82</v>
+      </c>
+      <c r="B30" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="C30" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="D30" s="29" t="s">
+        <v>354</v>
+      </c>
+      <c r="E30" s="27" t="s">
+        <v>354</v>
+      </c>
+      <c r="F30" s="18" t="s">
+        <v>354</v>
+      </c>
+      <c r="G30" s="18"/>
+      <c r="H30" s="27" t="s">
+        <v>189</v>
+      </c>
+      <c r="I30" s="27" t="s">
+        <v>391</v>
+      </c>
+      <c r="J30" s="27" t="s">
+        <v>391</v>
+      </c>
+      <c r="K30" s="27" t="s">
+        <v>391</v>
+      </c>
+      <c r="L30" s="27" t="s">
+        <v>391</v>
+      </c>
+      <c r="M30" s="18" t="s">
+        <v>391</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A31" s="27" t="s">
+        <v>85</v>
+      </c>
+      <c r="B31" s="27"/>
+      <c r="C31" s="32" t="s">
+        <v>355</v>
+      </c>
+      <c r="D31" s="35" t="s">
+        <v>559</v>
+      </c>
+      <c r="E31" s="32" t="s">
+        <v>560</v>
+      </c>
+      <c r="F31" s="18" t="s">
+        <v>559</v>
+      </c>
+      <c r="G31" s="18"/>
+      <c r="H31" s="27" t="s">
+        <v>192</v>
+      </c>
+      <c r="I31" s="33" t="s">
+        <v>585</v>
+      </c>
+      <c r="J31" s="27" t="s">
+        <v>392</v>
+      </c>
+      <c r="K31" s="29" t="s">
+        <v>607</v>
+      </c>
+      <c r="L31" s="33" t="s">
+        <v>585</v>
+      </c>
+      <c r="M31" s="18" t="s">
+        <v>392</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A32" s="27" t="s">
+        <v>88</v>
+      </c>
+      <c r="B32" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="C32" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="D32" s="27" t="s">
+        <v>356</v>
+      </c>
+      <c r="E32" s="30" t="s">
+        <v>561</v>
+      </c>
+      <c r="F32" s="18" t="s">
+        <v>356</v>
+      </c>
+      <c r="G32" s="18"/>
+      <c r="H32" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="I32" s="30" t="s">
+        <v>586</v>
+      </c>
+      <c r="J32" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="K32" s="30" t="s">
+        <v>608</v>
+      </c>
+      <c r="L32" s="27" t="s">
+        <v>393</v>
+      </c>
+      <c r="M32" s="18" t="s">
+        <v>744</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A33" s="27" t="s">
+        <v>91</v>
+      </c>
+      <c r="B33" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>357</v>
+      </c>
+      <c r="E33" s="30" t="s">
+        <v>562</v>
+      </c>
+      <c r="F33" s="18" t="s">
+        <v>357</v>
+      </c>
+      <c r="G33" s="18"/>
+      <c r="H33" s="27" t="s">
+        <v>198</v>
+      </c>
+      <c r="I33" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="J33" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="K33" s="36" t="s">
+        <v>760</v>
+      </c>
+      <c r="L33" s="27" t="s">
+        <v>394</v>
+      </c>
+      <c r="M33" s="18" t="s">
+        <v>755</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A34" s="27" t="s">
+        <v>94</v>
+      </c>
+      <c r="B34" s="27" t="s">
+        <v>358</v>
+      </c>
+      <c r="C34" s="30" t="s">
+        <v>358</v>
+      </c>
+      <c r="D34" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="E34" s="27" t="s">
+        <v>563</v>
+      </c>
+      <c r="F34" s="18" t="s">
+        <v>563</v>
+      </c>
+      <c r="G34" s="18"/>
+      <c r="H34" s="27" t="s">
+        <v>201</v>
+      </c>
+      <c r="I34" s="27" t="s">
+        <v>395</v>
+      </c>
+      <c r="J34" s="27" t="s">
+        <v>395</v>
+      </c>
+      <c r="K34" s="27" t="s">
+        <v>610</v>
+      </c>
+      <c r="L34" s="27" t="s">
+        <v>395</v>
+      </c>
+      <c r="M34" s="18" t="s">
+        <v>610</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A35" s="27" t="s">
+        <v>97</v>
+      </c>
+      <c r="B35" s="27" t="s">
+        <v>564</v>
+      </c>
+      <c r="C35" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="D35" s="27" t="s">
+        <v>590</v>
+      </c>
+      <c r="E35" s="27" t="s">
+        <v>359</v>
+      </c>
+      <c r="F35" s="18" t="s">
+        <v>590</v>
+      </c>
+      <c r="G35" s="18"/>
+      <c r="H35" s="27" t="s">
+        <v>204</v>
+      </c>
+      <c r="I35" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="J35" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="K35" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="L35" s="27" t="s">
+        <v>396</v>
+      </c>
+      <c r="M35" s="18" t="s">
+        <v>396</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A36" s="27" t="s">
+        <v>100</v>
+      </c>
+      <c r="B36" s="33" t="s">
+        <v>565</v>
+      </c>
+      <c r="C36" s="27" t="s">
+        <v>360</v>
+      </c>
+      <c r="D36" s="27" t="s">
+        <v>593</v>
+      </c>
+      <c r="E36" s="33" t="s">
+        <v>565</v>
+      </c>
+      <c r="F36" s="18" t="s">
+        <v>360</v>
+      </c>
+      <c r="G36" s="18"/>
+      <c r="H36" s="27" t="s">
+        <v>207</v>
+      </c>
+      <c r="I36" s="30" t="s">
+        <v>587</v>
+      </c>
+      <c r="J36" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="K36" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="L36" s="27" t="s">
+        <v>397</v>
+      </c>
+      <c r="M36" s="18" t="s">
+        <v>397</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A37" s="27" t="s">
+        <v>103</v>
+      </c>
+      <c r="B37" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="C37" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="D37" s="27" t="s">
+        <v>594</v>
+      </c>
+      <c r="E37" s="27" t="s">
+        <v>361</v>
+      </c>
+      <c r="F37" s="18" t="s">
+        <v>594</v>
+      </c>
+      <c r="G37" s="18"/>
+      <c r="H37" s="27" t="s">
+        <v>210</v>
+      </c>
+      <c r="I37" s="27"/>
+      <c r="J37" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="K37" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="L37" s="27" t="s">
+        <v>398</v>
+      </c>
+      <c r="M37" s="18" t="s">
+        <v>398</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="A38" s="27" t="s">
+        <v>106</v>
+      </c>
+      <c r="B38" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="C38" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="D38" s="27" t="s">
+        <v>595</v>
+      </c>
+      <c r="E38" s="27" t="s">
+        <v>362</v>
+      </c>
+      <c r="F38" s="18" t="s">
+        <v>595</v>
+      </c>
+      <c r="G38" s="18"/>
+      <c r="H38" s="27" t="s">
+        <v>213</v>
+      </c>
+      <c r="I38" s="30" t="s">
+        <v>589</v>
+      </c>
+      <c r="J38" s="27"/>
+      <c r="K38" s="27" t="s">
+        <v>588</v>
+      </c>
+      <c r="L38" s="27" t="s">
+        <v>588</v>
+      </c>
+      <c r="M38" s="18" t="s">
+        <v>588</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" ht="14.4" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A39" s="37" t="s">
+        <v>109</v>
+      </c>
+      <c r="B39" s="38" t="s">
+        <v>566</v>
+      </c>
+      <c r="C39" s="37" t="s">
+        <v>363</v>
+      </c>
+      <c r="D39" s="39" t="s">
+        <v>363</v>
+      </c>
+      <c r="E39" s="40"/>
+      <c r="F39" s="39" t="s">
+        <v>363</v>
+      </c>
+      <c r="G39" s="18"/>
+      <c r="H39" s="37"/>
+      <c r="I39" s="37"/>
+      <c r="J39" s="37"/>
+      <c r="K39" s="37"/>
+      <c r="L39" s="37"/>
+      <c r="M39" s="39"/>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G40" s="18"/>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G41" s="18"/>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G42" s="18"/>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G43" s="18"/>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G44" s="18"/>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G45" s="18"/>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G46" s="18"/>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G47" s="18"/>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="G48" s="18"/>
+    </row>
+    <row r="49" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G49" s="18"/>
+    </row>
+    <row r="50" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G50" s="18"/>
+    </row>
+    <row r="51" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G51" s="18"/>
+    </row>
+    <row r="52" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G52" s="18"/>
+    </row>
+    <row r="53" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G53" s="18"/>
+    </row>
+    <row r="54" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G54" s="18"/>
+    </row>
+    <row r="55" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G55" s="18"/>
+    </row>
+    <row r="56" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G56" s="18"/>
+    </row>
+    <row r="57" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G57" s="18"/>
+    </row>
+    <row r="58" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G58" s="18"/>
+    </row>
+    <row r="59" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G59" s="18"/>
+    </row>
+    <row r="60" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G60" s="18"/>
+    </row>
+    <row r="61" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G61" s="18"/>
+    </row>
+    <row r="62" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G62" s="18"/>
+    </row>
+    <row r="63" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G63" s="18"/>
+    </row>
+    <row r="64" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G64" s="18"/>
+    </row>
+    <row r="65" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G65" s="18"/>
+    </row>
+    <row r="66" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G66" s="18"/>
+    </row>
+    <row r="67" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G67" s="18"/>
+    </row>
+    <row r="68" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G68" s="18"/>
+    </row>
+    <row r="69" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G69" s="18"/>
+    </row>
+    <row r="70" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G70" s="18"/>
+    </row>
+    <row r="71" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G71" s="18"/>
+    </row>
+    <row r="72" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G72" s="18"/>
+    </row>
+    <row r="73" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G73" s="18"/>
+    </row>
+    <row r="74" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G74" s="18"/>
+    </row>
+    <row r="75" spans="7:7" x14ac:dyDescent="0.25">
+      <c r="G75" s="18"/>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="A1:A2"/>
+    <mergeCell ref="H1:H2"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="I1:M1"/>
+  </mergeCells>
+  <phoneticPr fontId="18" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>